<commit_message>
Update examples to use the WorkbookLocation() function
</commit_message>
<xml_diff>
--- a/basics/keyword_args.xlsx
+++ b/basics/keyword_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40C852D-1012-4879-8F9C-D53C906DEF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550530F8-DEA5-43C2-A4B6-33480CBB0F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2203" yWindow="4457" windowWidth="29426" windowHeight="13149" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -628,8 +628,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="str" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">LEFT(CELL("filename",B1),FIND("[",CELL("filename",B1))-1)</f>
-        <v>D:\github\xlslim-code-samples\basics\</v>
+        <f t="array" ref="B1">_xll.WorkbookLocation()</f>
+        <v>D:\github\xlslim-code-samples\basics</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -638,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f ca="1">B1&amp;"keyword_args.py"</f>
+        <f>B1&amp;"\keyword_args.py"</f>
         <v>D:\github\xlslim-code-samples\basics\keyword_args.py</v>
       </c>
       <c r="G2" s="1"/>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">_xll.RegisterPyModule(B2)</f>
+        <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
         <v>Registered D:\github\xlslim-code-samples\basics\keyword_args.py</v>
       </c>
       <c r="G3" s="1"/>
@@ -865,6 +865,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3725108ba1e248dd961cbde49d36f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a034177a2e5a667d336d2ca3036430" ns3:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -996,22 +1011,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C9D94B-68A3-4C5A-8543-29DBB1AA8066}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1027,28 +1051,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>